<commit_message>
R C R e2e
</commit_message>
<xml_diff>
--- a/E2EUAT.xlsx
+++ b/E2EUAT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="857" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="857" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="DatosRegresion" sheetId="25" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="457">
   <si>
     <t>N.º Documento</t>
   </si>
@@ -467,9 +467,6 @@
   </si>
   <si>
     <t>38452795</t>
-  </si>
-  <si>
-    <t>19006577</t>
   </si>
   <si>
     <t>59885133</t>
@@ -2914,7 +2911,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="211" customFormat="1" ht="15.6">
       <c r="A1" s="209" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B1" s="210" t="s">
         <v>16</v>
@@ -2944,7 +2941,7 @@
         <v>14</v>
       </c>
       <c r="K1" s="210" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L1" s="210" t="s">
         <v>123</v>
@@ -2956,42 +2953,42 @@
         <v>125</v>
       </c>
       <c r="O1" s="210" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="19.8" customHeight="1">
       <c r="A2" s="212" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B2" s="91" t="s">
+        <v>411</v>
+      </c>
+      <c r="C2" s="115" t="s">
         <v>412</v>
       </c>
-      <c r="C2" s="115" t="s">
-        <v>413</v>
-      </c>
       <c r="D2" s="90" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E2" s="90" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F2" s="90" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="91" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H2" s="92" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I2" s="90" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="90" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K2" s="90" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L2" s="90" t="s">
         <v>33</v>
@@ -3000,35 +2997,35 @@
         <v>34</v>
       </c>
       <c r="N2" s="177" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="O2" s="90" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="214" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B3" s="115" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C3" s="91" t="s">
+        <v>324</v>
+      </c>
+      <c r="D3" s="90" t="s">
         <v>325</v>
       </c>
-      <c r="D3" s="90" t="s">
+      <c r="E3" s="90" t="s">
         <v>326</v>
-      </c>
-      <c r="E3" s="90" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.6">
       <c r="A4" s="215" t="s">
+        <v>328</v>
+      </c>
+      <c r="B4" s="95" t="s">
         <v>329</v>
-      </c>
-      <c r="B4" s="95" t="s">
-        <v>330</v>
       </c>
       <c r="C4" s="95" t="s">
         <v>86</v>
@@ -3037,7 +3034,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="216" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F4" s="216" t="s">
         <v>88</v>
@@ -3052,41 +3049,41 @@
         <v>90</v>
       </c>
       <c r="J4" s="216" t="s">
+        <v>331</v>
+      </c>
+      <c r="K4" s="216" t="s">
         <v>332</v>
-      </c>
-      <c r="K4" s="216" t="s">
-        <v>333</v>
       </c>
       <c r="L4" s="216" t="s">
         <v>93</v>
       </c>
       <c r="M4" s="216" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N4" s="217"/>
       <c r="O4" s="217"/>
     </row>
     <row r="5" spans="1:15" ht="15">
       <c r="A5" s="218" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B5" s="91" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C5" s="69" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D5" s="91" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E5" s="219" t="s">
+        <v>213</v>
+      </c>
+      <c r="F5" s="219" t="s">
         <v>214</v>
       </c>
-      <c r="F5" s="219" t="s">
-        <v>215</v>
-      </c>
       <c r="G5" s="220" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H5" s="177" t="s">
         <v>39</v>
@@ -3104,17 +3101,17 @@
         <v>38</v>
       </c>
       <c r="M5" s="222" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N5" s="223"/>
       <c r="O5" s="223"/>
     </row>
     <row r="6" spans="1:15" ht="15.6">
       <c r="A6" s="215" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B6" s="95" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C6" s="216" t="s">
         <v>16</v>
@@ -3123,7 +3120,7 @@
         <v>98</v>
       </c>
       <c r="E6" s="216" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F6" s="216" t="s">
         <v>88</v>
@@ -3138,48 +3135,48 @@
         <v>90</v>
       </c>
       <c r="J6" s="216" t="s">
+        <v>331</v>
+      </c>
+      <c r="K6" s="216" t="s">
         <v>332</v>
-      </c>
-      <c r="K6" s="216" t="s">
-        <v>333</v>
       </c>
       <c r="L6" s="216" t="s">
         <v>93</v>
       </c>
       <c r="M6" s="216" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N6" s="217"/>
       <c r="O6" s="217"/>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="214" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B7" s="91" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C7" s="91" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D7" s="224" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="N7" s="223"/>
       <c r="O7" s="223"/>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="214" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B8" s="91" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C8" s="91" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D8" s="224" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E8" s="220"/>
       <c r="F8" s="177"/>
@@ -3195,25 +3192,25 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="214" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B9" s="91" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C9" s="91" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D9" s="224" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E9" s="219" t="s">
+        <v>213</v>
+      </c>
+      <c r="F9" s="177" t="s">
         <v>214</v>
       </c>
-      <c r="F9" s="177" t="s">
-        <v>215</v>
-      </c>
       <c r="G9" s="220" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H9" s="177" t="s">
         <v>39</v>
@@ -3231,14 +3228,14 @@
         <v>38</v>
       </c>
       <c r="M9" s="222" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N9" s="223"/>
       <c r="O9" s="223"/>
     </row>
     <row r="10" spans="1:15" ht="15.6">
       <c r="A10" s="215" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B10" s="94" t="s">
         <v>0</v>
@@ -3247,7 +3244,7 @@
         <v>16</v>
       </c>
       <c r="D10" s="225" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E10" s="95" t="s">
         <v>87</v>
@@ -3281,53 +3278,53 @@
     </row>
     <row r="11" spans="1:15" ht="15">
       <c r="A11" s="214" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B11" s="91" t="s">
+        <v>406</v>
+      </c>
+      <c r="C11" s="91" t="s">
         <v>407</v>
       </c>
-      <c r="C11" s="91" t="s">
+      <c r="D11" s="227" t="s">
         <v>408</v>
-      </c>
-      <c r="D11" s="227" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15">
       <c r="A12" s="214" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B12" s="91" t="s">
+        <v>406</v>
+      </c>
+      <c r="C12" s="91" t="s">
         <v>407</v>
       </c>
-      <c r="C12" s="91" t="s">
+      <c r="D12" s="227" t="s">
         <v>408</v>
-      </c>
-      <c r="D12" s="227" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15">
       <c r="A13" s="214" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B13" s="91" t="s">
+        <v>406</v>
+      </c>
+      <c r="C13" s="91" t="s">
         <v>407</v>
       </c>
-      <c r="C13" s="91" t="s">
+      <c r="D13" s="227" t="s">
         <v>408</v>
       </c>
-      <c r="D13" s="227" t="s">
-        <v>409</v>
-      </c>
       <c r="E13" s="219" t="s">
+        <v>213</v>
+      </c>
+      <c r="F13" s="177" t="s">
         <v>214</v>
       </c>
-      <c r="F13" s="177" t="s">
-        <v>215</v>
-      </c>
       <c r="G13" s="220" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H13" s="177" t="s">
         <v>39</v>
@@ -3345,7 +3342,7 @@
         <v>38</v>
       </c>
       <c r="M13" s="222" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -3962,7 +3959,7 @@
     </row>
     <row r="8" spans="1:5" ht="13.8" thickBot="1">
       <c r="A8" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B8" s="188">
         <v>22222035</v>
@@ -3975,7 +3972,7 @@
     </row>
     <row r="9" spans="1:5" ht="13.8" thickBot="1">
       <c r="A9" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9" s="178">
         <v>38010576</v>
@@ -3990,7 +3987,7 @@
     </row>
     <row r="10" spans="1:5" ht="13.8" thickBot="1">
       <c r="A10" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B10" s="178">
         <v>38010576</v>
@@ -4005,7 +4002,7 @@
     </row>
     <row r="11" spans="1:5" ht="13.8" thickBot="1">
       <c r="A11" s="31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B11" s="178">
         <v>38010576</v>
@@ -4020,7 +4017,7 @@
     </row>
     <row r="12" spans="1:5" ht="13.8" thickBot="1">
       <c r="A12" s="31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B12" s="178">
         <v>38010576</v>
@@ -4035,7 +4032,7 @@
     </row>
     <row r="13" spans="1:5" ht="13.8" thickBot="1">
       <c r="A13" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B13" s="178">
         <v>38010576</v>
@@ -4050,7 +4047,7 @@
     </row>
     <row r="14" spans="1:5" ht="13.8" thickBot="1">
       <c r="A14" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B14" s="178">
         <v>38010576</v>
@@ -4172,10 +4169,10 @@
         <v>83</v>
       </c>
       <c r="B2" s="68" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C2" s="68" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D2" s="75"/>
       <c r="E2" s="74"/>
@@ -4199,10 +4196,10 @@
         <v>134</v>
       </c>
       <c r="B3" s="68" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C3" s="68" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D3" s="75"/>
       <c r="E3" s="74"/>
@@ -4223,13 +4220,13 @@
     </row>
     <row r="4" spans="1:19" s="21" customFormat="1" ht="15.6" thickBot="1">
       <c r="A4" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" s="78" t="s">
         <v>209</v>
       </c>
-      <c r="B4" s="78" t="s">
-        <v>210</v>
-      </c>
       <c r="C4" s="69" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D4" s="75"/>
       <c r="E4" s="74"/>
@@ -4250,49 +4247,49 @@
     </row>
     <row r="5" spans="1:19" ht="15.6" thickBot="1">
       <c r="A5" s="24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B5" s="78" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C5" s="69" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D5" s="79" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E5" s="80" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="79" t="s">
+        <v>211</v>
+      </c>
+      <c r="G5" s="72" t="s">
         <v>212</v>
       </c>
-      <c r="G5" s="72" t="s">
+      <c r="H5" s="72" t="s">
         <v>213</v>
       </c>
-      <c r="H5" s="72" t="s">
+      <c r="I5" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="J5" s="72" t="s">
         <v>215</v>
-      </c>
-      <c r="J5" s="72" t="s">
-        <v>216</v>
       </c>
       <c r="K5" s="18" t="s">
         <v>39</v>
       </c>
       <c r="L5" s="71" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M5" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N5" s="18" t="s">
         <v>62</v>
       </c>
       <c r="O5" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P5" s="81" t="s">
         <v>20</v>
@@ -4301,28 +4298,28 @@
         <v>33332010</v>
       </c>
       <c r="R5" s="244" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="S5" s="245"/>
     </row>
     <row r="6" spans="1:19" ht="15">
       <c r="A6" s="65" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B6" s="78" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C6" s="69" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D6" s="79" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E6" s="80" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="79" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -4355,18 +4352,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.6">
       <c r="A1" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>236</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>238</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -4394,37 +4391,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16.2" thickBot="1">
       <c r="A1" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="C1" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="D1" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="E1" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="F1" s="38" t="s">
         <v>244</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="G1" s="38" t="s">
         <v>245</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="H1" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="I1" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="J1" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="K1" s="38" t="s">
         <v>249</v>
-      </c>
-      <c r="K1" s="38" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.6" thickBot="1">
@@ -4546,25 +4543,25 @@
     </row>
     <row r="11" spans="1:11" ht="13.8" thickBot="1">
       <c r="A11" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="C11" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="C11" s="21" t="s">
-        <v>253</v>
-      </c>
       <c r="D11" s="208" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
       <c r="I11" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J11" s="21"/>
       <c r="K11" s="21"/>
@@ -4619,21 +4616,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.6">
       <c r="A1" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15">
       <c r="A2" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="35"/>
@@ -4641,16 +4638,16 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B3" s="46" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="D3" s="7" t="s">
         <v>256</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4721,59 +4718,59 @@
         <v>15</v>
       </c>
       <c r="K1" s="94" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L1" s="94" t="s">
         <v>123</v>
       </c>
       <c r="M1" s="94" t="s">
+        <v>271</v>
+      </c>
+      <c r="N1" s="94" t="s">
         <v>272</v>
       </c>
-      <c r="N1" s="94" t="s">
+      <c r="O1" s="94" t="s">
         <v>273</v>
-      </c>
-      <c r="O1" s="94" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.6">
       <c r="A2" s="136" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="90" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B3" s="115" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C3" s="115" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D3" s="90" t="s">
+        <v>316</v>
+      </c>
+      <c r="E3" s="90" t="s">
         <v>317</v>
       </c>
-      <c r="E3" s="90" t="s">
-        <v>318</v>
-      </c>
       <c r="F3" s="90" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G3" s="91" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H3" s="92" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I3" s="102" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="100" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K3" s="100" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L3" s="100" t="s">
         <v>33</v>
@@ -4782,24 +4779,24 @@
         <v>34</v>
       </c>
       <c r="N3" s="100" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="O3" s="103" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="90" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B4" s="115" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C4" s="137" t="s">
+        <v>301</v>
+      </c>
+      <c r="D4" s="90" t="s">
         <v>302</v>
-      </c>
-      <c r="D4" s="90" t="s">
-        <v>303</v>
       </c>
       <c r="E4" s="90" t="s">
         <v>57</v>
@@ -4817,40 +4814,40 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="90" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B5" s="115" t="s">
+        <v>318</v>
+      </c>
+      <c r="C5" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="C5" s="100" t="s">
-        <v>320</v>
-      </c>
       <c r="D5" s="90" t="s">
+        <v>291</v>
+      </c>
+      <c r="E5" s="90" t="s">
         <v>292</v>
-      </c>
-      <c r="E5" s="90" t="s">
-        <v>293</v>
       </c>
       <c r="F5" s="90" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="91" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H5" s="102" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I5" s="92" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J5" s="90" t="s">
         <v>13</v>
       </c>
       <c r="K5" s="90" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L5" s="90" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M5" s="90" t="s">
         <v>33</v>
@@ -4859,24 +4856,24 @@
         <v>34</v>
       </c>
       <c r="O5" s="100" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P5" s="90" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="90" t="s">
+        <v>196</v>
+      </c>
+      <c r="B6" s="91" t="s">
         <v>197</v>
       </c>
-      <c r="B6" s="91" t="s">
+      <c r="C6" s="91" t="s">
         <v>198</v>
       </c>
-      <c r="C6" s="91" t="s">
+      <c r="D6" s="91" t="s">
         <v>199</v>
-      </c>
-      <c r="D6" s="91" t="s">
-        <v>200</v>
       </c>
       <c r="E6" s="91" t="s">
         <v>57</v>
@@ -4885,16 +4882,16 @@
         <v>10</v>
       </c>
       <c r="G6" s="91" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H6" s="123" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I6" s="91" t="s">
         <v>13</v>
       </c>
       <c r="J6" s="91" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K6" s="91" t="s">
         <v>33</v>
@@ -4909,19 +4906,19 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="90" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B7" s="115" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C7" s="115" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D7" s="90" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="102" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F7" s="90"/>
       <c r="G7" s="90"/>
@@ -4935,21 +4932,21 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="98" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B8" s="115" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C8" s="115" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="98" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B9" s="102" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C9" s="102">
         <v>16552744</v>
@@ -4957,42 +4954,42 @@
     </row>
     <row r="10" spans="1:16" ht="15.6">
       <c r="A10" s="136" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="90" t="s">
+        <v>194</v>
+      </c>
+      <c r="B11" s="115" t="s">
+        <v>299</v>
+      </c>
+      <c r="C11" s="115" t="s">
+        <v>301</v>
+      </c>
+      <c r="D11" s="90" t="s">
+        <v>300</v>
+      </c>
+      <c r="E11" s="90" t="s">
+        <v>296</v>
+      </c>
+      <c r="F11" s="90" t="s">
+        <v>269</v>
+      </c>
+      <c r="G11" s="91" t="s">
         <v>195</v>
       </c>
-      <c r="B11" s="115" t="s">
-        <v>300</v>
-      </c>
-      <c r="C11" s="115" t="s">
-        <v>302</v>
-      </c>
-      <c r="D11" s="90" t="s">
-        <v>301</v>
-      </c>
-      <c r="E11" s="90" t="s">
-        <v>297</v>
-      </c>
-      <c r="F11" s="90" t="s">
-        <v>270</v>
-      </c>
-      <c r="G11" s="91" t="s">
-        <v>196</v>
-      </c>
       <c r="H11" s="92" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I11" s="102" t="s">
         <v>13</v>
       </c>
       <c r="J11" s="100" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K11" s="100" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L11" s="100" t="s">
         <v>33</v>
@@ -5001,18 +4998,18 @@
         <v>34</v>
       </c>
       <c r="N11" s="100" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="O11" s="103" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="98" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B12" s="102" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C12" s="102">
         <v>22355504</v>
@@ -5020,13 +5017,13 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="98" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B13" s="115" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C13" s="115" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D13" s="98" t="s">
         <v>10</v>
@@ -5035,33 +5032,33 @@
         <v>33649</v>
       </c>
       <c r="F13" s="98" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="98" t="s">
+        <v>284</v>
+      </c>
+      <c r="B14" s="115" t="s">
+        <v>299</v>
+      </c>
+      <c r="C14" s="115" t="s">
+        <v>315</v>
+      </c>
+      <c r="D14" s="99" t="s">
+        <v>293</v>
+      </c>
+      <c r="E14" s="98" t="s">
         <v>285</v>
-      </c>
-      <c r="B14" s="115" t="s">
-        <v>300</v>
-      </c>
-      <c r="C14" s="115" t="s">
-        <v>316</v>
-      </c>
-      <c r="D14" s="99" t="s">
-        <v>294</v>
-      </c>
-      <c r="E14" s="98" t="s">
-        <v>286</v>
       </c>
       <c r="F14" s="98" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="91" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H14" s="139" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I14" s="138">
         <v>45703</v>
@@ -5069,28 +5066,28 @@
     </row>
     <row r="15" spans="1:16" ht="15.6">
       <c r="A15" s="136" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B15" s="115" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C15" s="115" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D15" s="91" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" s="91" t="s">
         <v>189</v>
-      </c>
-      <c r="E15" s="91" t="s">
-        <v>190</v>
       </c>
       <c r="F15" s="130" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="91" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H15" s="123" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I15" s="91"/>
       <c r="J15" s="91"/>
@@ -5101,16 +5098,16 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="90" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B16" s="115" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C16" s="115" t="s">
+        <v>301</v>
+      </c>
+      <c r="D16" s="90" t="s">
         <v>302</v>
-      </c>
-      <c r="D16" s="90" t="s">
-        <v>303</v>
       </c>
       <c r="E16" s="90" t="s">
         <v>57</v>
@@ -5119,19 +5116,19 @@
         <v>10</v>
       </c>
       <c r="G16" s="91" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H16" s="92" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I16" s="102" t="s">
         <v>13</v>
       </c>
       <c r="J16" s="100" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K16" s="100" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L16" s="100" t="s">
         <v>33</v>
@@ -5140,41 +5137,41 @@
         <v>34</v>
       </c>
       <c r="N16" s="100" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="O16" s="103" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="98" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="90" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B18" s="115" t="s">
+        <v>299</v>
+      </c>
+      <c r="C18" s="115" t="s">
+        <v>301</v>
+      </c>
+      <c r="D18" s="90" t="s">
         <v>300</v>
       </c>
-      <c r="C18" s="115" t="s">
-        <v>302</v>
-      </c>
-      <c r="D18" s="90" t="s">
-        <v>301</v>
-      </c>
       <c r="E18" s="90" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F18" s="90" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G18" s="91" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H18" s="92" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I18" s="90"/>
       <c r="J18" s="90"/>
@@ -5188,49 +5185,49 @@
         <v>2932598064</v>
       </c>
       <c r="B19" s="141" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C19" s="141" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D19" s="141" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E19" s="141" t="s">
         <v>10</v>
       </c>
       <c r="F19" s="142" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G19" s="143" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H19" s="141" t="s">
         <v>13</v>
       </c>
       <c r="I19" s="141" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="J19" s="141" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K19" s="141" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L19" s="141" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M19" s="144" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="N19" s="141" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O19" s="141" t="s">
         <v>61</v>
       </c>
       <c r="P19" s="141" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="31.2">
@@ -5263,30 +5260,30 @@
         <v>15</v>
       </c>
       <c r="K21" s="94" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L21" s="94" t="s">
         <v>123</v>
       </c>
       <c r="M21" s="94" t="s">
+        <v>271</v>
+      </c>
+      <c r="N21" s="94" t="s">
         <v>272</v>
       </c>
-      <c r="N21" s="94" t="s">
+      <c r="O21" s="94" t="s">
         <v>273</v>
       </c>
-      <c r="O21" s="94" t="s">
-        <v>274</v>
-      </c>
       <c r="P21" s="133" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q21" s="133" t="s">
         <v>366</v>
-      </c>
-      <c r="Q21" s="133" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="14.4">
       <c r="A22" s="88" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B22" s="146"/>
       <c r="C22" s="34"/>
@@ -5309,7 +5306,7 @@
     </row>
     <row r="23" spans="1:20" s="114" customFormat="1" ht="14.4">
       <c r="A23" s="88" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B23" s="146"/>
       <c r="C23" s="34"/>
@@ -5332,7 +5329,7 @@
     </row>
     <row r="24" spans="1:20" s="114" customFormat="1" ht="14.4" customHeight="1">
       <c r="A24" s="88" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B24" s="146"/>
       <c r="C24" s="34"/>
@@ -5355,7 +5352,7 @@
     </row>
     <row r="25" spans="1:20" s="114" customFormat="1" ht="14.4">
       <c r="A25" s="88" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B25" s="146"/>
       <c r="C25" s="34"/>
@@ -5378,7 +5375,7 @@
     </row>
     <row r="26" spans="1:20" s="114" customFormat="1" ht="14.4">
       <c r="A26" s="88" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B26" s="146"/>
       <c r="C26" s="34"/>
@@ -5401,7 +5398,7 @@
     </row>
     <row r="27" spans="1:20" s="114" customFormat="1" ht="14.4">
       <c r="A27" s="88" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B27" s="146"/>
       <c r="C27" s="34"/>
@@ -5424,7 +5421,7 @@
     </row>
     <row r="28" spans="1:20" s="114" customFormat="1" ht="14.4">
       <c r="A28" s="88" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B28" s="147"/>
       <c r="C28" s="34"/>
@@ -5447,7 +5444,7 @@
     </row>
     <row r="29" spans="1:20" s="156" customFormat="1" ht="14.4">
       <c r="A29" s="88" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B29" s="147"/>
       <c r="C29" s="34"/>
@@ -5470,7 +5467,7 @@
     </row>
     <row r="30" spans="1:20" s="156" customFormat="1" ht="14.4">
       <c r="A30" s="88" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B30" s="147"/>
       <c r="C30" s="34"/>
@@ -5493,7 +5490,7 @@
     </row>
     <row r="31" spans="1:20" s="156" customFormat="1" ht="14.4">
       <c r="A31" s="88" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B31" s="147"/>
       <c r="C31" s="34"/>
@@ -5516,7 +5513,7 @@
     </row>
     <row r="32" spans="1:20" s="156" customFormat="1" ht="14.4">
       <c r="A32" s="88" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B32" s="147"/>
       <c r="C32" s="34"/>
@@ -5539,7 +5536,7 @@
     </row>
     <row r="33" spans="1:20" s="156" customFormat="1" ht="14.4">
       <c r="A33" s="88" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B33" s="147"/>
       <c r="C33" s="34"/>
@@ -5562,7 +5559,7 @@
     </row>
     <row r="34" spans="1:20" s="156" customFormat="1" ht="14.4">
       <c r="A34" s="88" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B34" s="147"/>
       <c r="C34" s="34"/>
@@ -5585,7 +5582,7 @@
     </row>
     <row r="35" spans="1:20" s="156" customFormat="1" ht="14.4">
       <c r="A35" s="88" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B35" s="160"/>
       <c r="C35" s="34"/>
@@ -5608,7 +5605,7 @@
     </row>
     <row r="36" spans="1:20" ht="14.4">
       <c r="A36" s="88" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B36" s="147"/>
       <c r="C36" s="34"/>
@@ -5682,652 +5679,652 @@
         <v>15</v>
       </c>
       <c r="K42" s="95" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L42" s="95" t="s">
         <v>123</v>
       </c>
       <c r="M42" s="95" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N42" s="95" t="s">
         <v>125</v>
       </c>
       <c r="O42" s="96" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P42" s="132" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q42" s="133" t="s">
         <v>365</v>
       </c>
-      <c r="Q42" s="133" t="s">
+      <c r="R42" s="133" t="s">
         <v>366</v>
       </c>
-      <c r="R42" s="133" t="s">
+      <c r="S42" s="133" t="s">
         <v>367</v>
       </c>
-      <c r="S42" s="133" t="s">
+      <c r="T42" s="133" t="s">
         <v>368</v>
-      </c>
-      <c r="T42" s="133" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="43" spans="1:20" s="156" customFormat="1" ht="14.4">
       <c r="A43" s="197"/>
       <c r="B43" s="198" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C43" s="175" t="s">
+        <v>382</v>
+      </c>
+      <c r="D43" s="112" t="s">
         <v>383</v>
       </c>
-      <c r="D43" s="112" t="s">
-        <v>384</v>
-      </c>
       <c r="E43" s="99" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F43" s="99" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G43" s="91" t="s">
+        <v>375</v>
+      </c>
+      <c r="H43" s="176" t="s">
+        <v>353</v>
+      </c>
+      <c r="I43" s="100" t="s">
+        <v>377</v>
+      </c>
+      <c r="J43" s="100" t="s">
         <v>376</v>
       </c>
-      <c r="H43" s="176" t="s">
-        <v>354</v>
-      </c>
-      <c r="I43" s="100" t="s">
+      <c r="K43" s="89" t="s">
+        <v>275</v>
+      </c>
+      <c r="L43" s="99" t="s">
+        <v>380</v>
+      </c>
+      <c r="M43" s="100" t="s">
+        <v>373</v>
+      </c>
+      <c r="N43" s="177" t="s">
         <v>378</v>
       </c>
-      <c r="J43" s="100" t="s">
-        <v>377</v>
-      </c>
-      <c r="K43" s="89" t="s">
-        <v>276</v>
-      </c>
-      <c r="L43" s="99" t="s">
-        <v>381</v>
-      </c>
-      <c r="M43" s="100" t="s">
-        <v>374</v>
-      </c>
-      <c r="N43" s="177" t="s">
+      <c r="O43" s="103" t="s">
+        <v>370</v>
+      </c>
+      <c r="P43" s="99" t="s">
         <v>379</v>
-      </c>
-      <c r="O43" s="103" t="s">
-        <v>371</v>
-      </c>
-      <c r="P43" s="99" t="s">
-        <v>380</v>
       </c>
       <c r="Q43" s="100" t="s">
         <v>36</v>
       </c>
       <c r="R43" s="99" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S43" s="99" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="T43" s="100" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="44" spans="1:20" s="156" customFormat="1" ht="14.4">
       <c r="A44" s="99" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B44" s="199">
         <v>2932598371</v>
       </c>
       <c r="C44" s="175" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D44" s="112" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E44" s="99" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F44" s="99" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G44" s="91" t="s">
+        <v>375</v>
+      </c>
+      <c r="H44" s="176" t="s">
+        <v>353</v>
+      </c>
+      <c r="I44" s="100" t="s">
+        <v>377</v>
+      </c>
+      <c r="J44" s="100" t="s">
         <v>376</v>
       </c>
-      <c r="H44" s="176" t="s">
-        <v>354</v>
-      </c>
-      <c r="I44" s="100" t="s">
+      <c r="K44" s="89" t="s">
+        <v>275</v>
+      </c>
+      <c r="L44" s="99" t="s">
+        <v>380</v>
+      </c>
+      <c r="M44" s="100" t="s">
+        <v>373</v>
+      </c>
+      <c r="N44" s="177" t="s">
         <v>378</v>
       </c>
-      <c r="J44" s="100" t="s">
-        <v>377</v>
-      </c>
-      <c r="K44" s="89" t="s">
-        <v>276</v>
-      </c>
-      <c r="L44" s="99" t="s">
-        <v>381</v>
-      </c>
-      <c r="M44" s="100" t="s">
-        <v>374</v>
-      </c>
-      <c r="N44" s="177" t="s">
+      <c r="O44" s="103" t="s">
+        <v>370</v>
+      </c>
+      <c r="P44" s="99" t="s">
         <v>379</v>
-      </c>
-      <c r="O44" s="103" t="s">
-        <v>371</v>
-      </c>
-      <c r="P44" s="99" t="s">
-        <v>380</v>
       </c>
       <c r="Q44" s="100" t="s">
         <v>36</v>
       </c>
       <c r="R44" s="99" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S44" s="99" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="T44" s="100" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="45" spans="1:20" s="156" customFormat="1" ht="14.4">
       <c r="A45" s="99" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B45" s="200">
         <v>2932598372</v>
       </c>
       <c r="C45" s="175" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D45" s="112" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E45" s="99" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F45" s="99" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G45" s="91" t="s">
+        <v>375</v>
+      </c>
+      <c r="H45" s="176" t="s">
+        <v>353</v>
+      </c>
+      <c r="I45" s="100" t="s">
+        <v>377</v>
+      </c>
+      <c r="J45" s="100" t="s">
         <v>376</v>
       </c>
-      <c r="H45" s="176" t="s">
-        <v>354</v>
-      </c>
-      <c r="I45" s="100" t="s">
+      <c r="K45" s="89" t="s">
+        <v>275</v>
+      </c>
+      <c r="L45" s="99" t="s">
+        <v>380</v>
+      </c>
+      <c r="M45" s="100" t="s">
+        <v>373</v>
+      </c>
+      <c r="N45" s="177" t="s">
         <v>378</v>
       </c>
-      <c r="J45" s="100" t="s">
-        <v>377</v>
-      </c>
-      <c r="K45" s="89" t="s">
-        <v>276</v>
-      </c>
-      <c r="L45" s="99" t="s">
-        <v>381</v>
-      </c>
-      <c r="M45" s="100" t="s">
-        <v>374</v>
-      </c>
-      <c r="N45" s="177" t="s">
+      <c r="O45" s="103" t="s">
+        <v>370</v>
+      </c>
+      <c r="P45" s="99" t="s">
         <v>379</v>
-      </c>
-      <c r="O45" s="103" t="s">
-        <v>371</v>
-      </c>
-      <c r="P45" s="99" t="s">
-        <v>380</v>
       </c>
       <c r="Q45" s="100" t="s">
         <v>36</v>
       </c>
       <c r="R45" s="99" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S45" s="99" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="T45" s="100" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="46" spans="1:20" s="156" customFormat="1" ht="14.4">
       <c r="A46" s="99" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B46" s="200">
         <v>2932598373</v>
       </c>
       <c r="C46" s="175" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D46" s="112" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E46" s="99" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F46" s="99" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G46" s="91" t="s">
+        <v>375</v>
+      </c>
+      <c r="H46" s="176" t="s">
+        <v>353</v>
+      </c>
+      <c r="I46" s="100" t="s">
+        <v>377</v>
+      </c>
+      <c r="J46" s="100" t="s">
         <v>376</v>
       </c>
-      <c r="H46" s="176" t="s">
-        <v>354</v>
-      </c>
-      <c r="I46" s="100" t="s">
+      <c r="K46" s="89" t="s">
+        <v>275</v>
+      </c>
+      <c r="L46" s="99" t="s">
+        <v>380</v>
+      </c>
+      <c r="M46" s="100" t="s">
+        <v>373</v>
+      </c>
+      <c r="N46" s="177" t="s">
         <v>378</v>
       </c>
-      <c r="J46" s="100" t="s">
-        <v>377</v>
-      </c>
-      <c r="K46" s="89" t="s">
-        <v>276</v>
-      </c>
-      <c r="L46" s="99" t="s">
-        <v>381</v>
-      </c>
-      <c r="M46" s="100" t="s">
-        <v>374</v>
-      </c>
-      <c r="N46" s="177" t="s">
+      <c r="O46" s="103" t="s">
+        <v>370</v>
+      </c>
+      <c r="P46" s="99" t="s">
         <v>379</v>
-      </c>
-      <c r="O46" s="103" t="s">
-        <v>371</v>
-      </c>
-      <c r="P46" s="99" t="s">
-        <v>380</v>
       </c>
       <c r="Q46" s="100" t="s">
         <v>36</v>
       </c>
       <c r="R46" s="99" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S46" s="99" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="T46" s="100" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="47" spans="1:20" s="156" customFormat="1" ht="14.4">
       <c r="A47" s="99" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B47" s="200">
         <v>2932598374</v>
       </c>
       <c r="C47" s="175" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D47" s="112" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E47" s="99" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F47" s="99" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G47" s="91" t="s">
+        <v>375</v>
+      </c>
+      <c r="H47" s="176" t="s">
+        <v>353</v>
+      </c>
+      <c r="I47" s="100" t="s">
+        <v>377</v>
+      </c>
+      <c r="J47" s="100" t="s">
         <v>376</v>
       </c>
-      <c r="H47" s="176" t="s">
-        <v>354</v>
-      </c>
-      <c r="I47" s="100" t="s">
+      <c r="K47" s="89" t="s">
+        <v>275</v>
+      </c>
+      <c r="L47" s="99" t="s">
+        <v>380</v>
+      </c>
+      <c r="M47" s="100" t="s">
+        <v>373</v>
+      </c>
+      <c r="N47" s="177" t="s">
         <v>378</v>
       </c>
-      <c r="J47" s="100" t="s">
-        <v>377</v>
-      </c>
-      <c r="K47" s="89" t="s">
-        <v>276</v>
-      </c>
-      <c r="L47" s="99" t="s">
-        <v>381</v>
-      </c>
-      <c r="M47" s="100" t="s">
-        <v>374</v>
-      </c>
-      <c r="N47" s="177" t="s">
+      <c r="O47" s="103" t="s">
+        <v>370</v>
+      </c>
+      <c r="P47" s="99" t="s">
         <v>379</v>
-      </c>
-      <c r="O47" s="103" t="s">
-        <v>371</v>
-      </c>
-      <c r="P47" s="99" t="s">
-        <v>380</v>
       </c>
       <c r="Q47" s="100" t="s">
         <v>36</v>
       </c>
       <c r="R47" s="99" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S47" s="99" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="T47" s="100" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="48" spans="1:20" s="156" customFormat="1" ht="14.4">
       <c r="A48" s="99" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B48" s="200">
         <v>2932598375</v>
       </c>
       <c r="C48" s="175" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D48" s="112" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E48" s="99" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F48" s="99" t="s">
         <v>10</v>
       </c>
       <c r="G48" s="91" t="s">
+        <v>375</v>
+      </c>
+      <c r="H48" s="176" t="s">
+        <v>353</v>
+      </c>
+      <c r="I48" s="100" t="s">
+        <v>377</v>
+      </c>
+      <c r="J48" s="100" t="s">
         <v>376</v>
       </c>
-      <c r="H48" s="176" t="s">
-        <v>354</v>
-      </c>
-      <c r="I48" s="100" t="s">
+      <c r="K48" s="89" t="s">
+        <v>275</v>
+      </c>
+      <c r="L48" s="99" t="s">
+        <v>380</v>
+      </c>
+      <c r="M48" s="100" t="s">
+        <v>373</v>
+      </c>
+      <c r="N48" s="177" t="s">
         <v>378</v>
       </c>
-      <c r="J48" s="100" t="s">
-        <v>377</v>
-      </c>
-      <c r="K48" s="89" t="s">
-        <v>276</v>
-      </c>
-      <c r="L48" s="99" t="s">
-        <v>381</v>
-      </c>
-      <c r="M48" s="100" t="s">
-        <v>374</v>
-      </c>
-      <c r="N48" s="177" t="s">
+      <c r="O48" s="103" t="s">
+        <v>370</v>
+      </c>
+      <c r="P48" s="99" t="s">
         <v>379</v>
-      </c>
-      <c r="O48" s="103" t="s">
-        <v>371</v>
-      </c>
-      <c r="P48" s="99" t="s">
-        <v>380</v>
       </c>
       <c r="Q48" s="100" t="s">
         <v>36</v>
       </c>
       <c r="R48" s="99" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S48" s="99" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="T48" s="100" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="49" spans="1:20" s="156" customFormat="1" ht="14.4">
       <c r="A49" s="99" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B49" s="200">
         <v>2932598376</v>
       </c>
       <c r="C49" s="175" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D49" s="112" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E49" s="99" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F49" s="99" t="s">
         <v>10</v>
       </c>
       <c r="G49" s="91" t="s">
+        <v>375</v>
+      </c>
+      <c r="H49" s="176" t="s">
+        <v>353</v>
+      </c>
+      <c r="I49" s="100" t="s">
+        <v>377</v>
+      </c>
+      <c r="J49" s="100" t="s">
         <v>376</v>
       </c>
-      <c r="H49" s="176" t="s">
-        <v>354</v>
-      </c>
-      <c r="I49" s="100" t="s">
+      <c r="K49" s="89" t="s">
+        <v>275</v>
+      </c>
+      <c r="L49" s="99" t="s">
+        <v>380</v>
+      </c>
+      <c r="M49" s="100" t="s">
+        <v>373</v>
+      </c>
+      <c r="N49" s="177" t="s">
         <v>378</v>
       </c>
-      <c r="J49" s="100" t="s">
-        <v>377</v>
-      </c>
-      <c r="K49" s="89" t="s">
-        <v>276</v>
-      </c>
-      <c r="L49" s="99" t="s">
-        <v>381</v>
-      </c>
-      <c r="M49" s="100" t="s">
-        <v>374</v>
-      </c>
-      <c r="N49" s="177" t="s">
+      <c r="O49" s="103" t="s">
+        <v>370</v>
+      </c>
+      <c r="P49" s="99" t="s">
         <v>379</v>
-      </c>
-      <c r="O49" s="103" t="s">
-        <v>371</v>
-      </c>
-      <c r="P49" s="99" t="s">
-        <v>380</v>
       </c>
       <c r="Q49" s="100" t="s">
         <v>36</v>
       </c>
       <c r="R49" s="99" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S49" s="99" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="T49" s="100" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" spans="1:20" s="156" customFormat="1" ht="14.4">
       <c r="A50" s="99" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B50" s="200">
         <v>2932598377</v>
       </c>
       <c r="C50" s="175" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D50" s="112" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E50" s="99" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F50" s="99" t="s">
         <v>10</v>
       </c>
       <c r="G50" s="91" t="s">
+        <v>375</v>
+      </c>
+      <c r="H50" s="176" t="s">
+        <v>353</v>
+      </c>
+      <c r="I50" s="100" t="s">
+        <v>377</v>
+      </c>
+      <c r="J50" s="100" t="s">
         <v>376</v>
       </c>
-      <c r="H50" s="176" t="s">
-        <v>354</v>
-      </c>
-      <c r="I50" s="100" t="s">
+      <c r="K50" s="89" t="s">
+        <v>275</v>
+      </c>
+      <c r="L50" s="99" t="s">
+        <v>380</v>
+      </c>
+      <c r="M50" s="100" t="s">
+        <v>373</v>
+      </c>
+      <c r="N50" s="177" t="s">
         <v>378</v>
       </c>
-      <c r="J50" s="100" t="s">
-        <v>377</v>
-      </c>
-      <c r="K50" s="89" t="s">
-        <v>276</v>
-      </c>
-      <c r="L50" s="99" t="s">
-        <v>381</v>
-      </c>
-      <c r="M50" s="100" t="s">
-        <v>374</v>
-      </c>
-      <c r="N50" s="177" t="s">
+      <c r="O50" s="103" t="s">
+        <v>370</v>
+      </c>
+      <c r="P50" s="99" t="s">
         <v>379</v>
-      </c>
-      <c r="O50" s="103" t="s">
-        <v>371</v>
-      </c>
-      <c r="P50" s="99" t="s">
-        <v>380</v>
       </c>
       <c r="Q50" s="100" t="s">
         <v>36</v>
       </c>
       <c r="R50" s="99" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S50" s="99" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="T50" s="100" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="51" spans="1:20" s="156" customFormat="1" ht="14.4">
       <c r="A51" s="99" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B51" s="201">
         <v>2932598482</v>
       </c>
       <c r="C51" s="175" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D51" s="112" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E51" s="99" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F51" s="99" t="s">
         <v>10</v>
       </c>
       <c r="G51" s="91" t="s">
+        <v>375</v>
+      </c>
+      <c r="H51" s="176" t="s">
+        <v>353</v>
+      </c>
+      <c r="I51" s="100" t="s">
+        <v>377</v>
+      </c>
+      <c r="J51" s="100" t="s">
         <v>376</v>
       </c>
-      <c r="H51" s="176" t="s">
-        <v>354</v>
-      </c>
-      <c r="I51" s="100" t="s">
+      <c r="K51" s="89" t="s">
+        <v>275</v>
+      </c>
+      <c r="L51" s="99" t="s">
+        <v>380</v>
+      </c>
+      <c r="M51" s="100" t="s">
+        <v>373</v>
+      </c>
+      <c r="N51" s="177" t="s">
         <v>378</v>
       </c>
-      <c r="J51" s="100" t="s">
-        <v>377</v>
-      </c>
-      <c r="K51" s="89" t="s">
-        <v>276</v>
-      </c>
-      <c r="L51" s="99" t="s">
-        <v>381</v>
-      </c>
-      <c r="M51" s="100" t="s">
-        <v>374</v>
-      </c>
-      <c r="N51" s="177" t="s">
+      <c r="O51" s="103" t="s">
+        <v>370</v>
+      </c>
+      <c r="P51" s="99" t="s">
         <v>379</v>
-      </c>
-      <c r="O51" s="103" t="s">
-        <v>371</v>
-      </c>
-      <c r="P51" s="99" t="s">
-        <v>380</v>
       </c>
       <c r="Q51" s="100" t="s">
         <v>36</v>
       </c>
       <c r="R51" s="99" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S51" s="99" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="T51" s="100" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="52" spans="1:20" s="156" customFormat="1" ht="14.4">
       <c r="A52" s="99" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B52" s="201">
         <v>2932598441</v>
       </c>
       <c r="C52" s="175" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D52" s="112" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E52" s="99" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F52" s="99" t="s">
         <v>10</v>
       </c>
       <c r="G52" s="91" t="s">
+        <v>375</v>
+      </c>
+      <c r="H52" s="176" t="s">
+        <v>353</v>
+      </c>
+      <c r="I52" s="100" t="s">
+        <v>377</v>
+      </c>
+      <c r="J52" s="100" t="s">
         <v>376</v>
       </c>
-      <c r="H52" s="176" t="s">
-        <v>354</v>
-      </c>
-      <c r="I52" s="100" t="s">
+      <c r="K52" s="89" t="s">
+        <v>275</v>
+      </c>
+      <c r="L52" s="99" t="s">
+        <v>380</v>
+      </c>
+      <c r="M52" s="100" t="s">
+        <v>373</v>
+      </c>
+      <c r="N52" s="177" t="s">
         <v>378</v>
       </c>
-      <c r="J52" s="100" t="s">
-        <v>377</v>
-      </c>
-      <c r="K52" s="89" t="s">
-        <v>276</v>
-      </c>
-      <c r="L52" s="99" t="s">
-        <v>381</v>
-      </c>
-      <c r="M52" s="100" t="s">
-        <v>374</v>
-      </c>
-      <c r="N52" s="177" t="s">
+      <c r="O52" s="103" t="s">
+        <v>370</v>
+      </c>
+      <c r="P52" s="99" t="s">
         <v>379</v>
-      </c>
-      <c r="O52" s="103" t="s">
-        <v>371</v>
-      </c>
-      <c r="P52" s="99" t="s">
-        <v>380</v>
       </c>
       <c r="Q52" s="100" t="s">
         <v>36</v>
       </c>
       <c r="R52" s="99" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S52" s="99" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="T52" s="100" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="53" spans="1:20" s="156" customFormat="1" ht="14.4">
@@ -6936,49 +6933,49 @@
         <v>2932598206</v>
       </c>
       <c r="B140" s="149" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C140" s="149" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D140" s="149" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E140" s="149" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F140" s="150" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G140" s="151" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H140" s="149" t="s">
         <v>13</v>
       </c>
       <c r="I140" s="149" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J140" s="149" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K140" s="149" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="L140" s="149" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M140" s="149" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="N140" s="149" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O140" s="149" t="s">
         <v>61</v>
       </c>
       <c r="P140" s="149" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="141" spans="1:16" ht="15">
@@ -6986,49 +6983,49 @@
         <v>2932598207</v>
       </c>
       <c r="B141" s="153" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C141" s="153" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D141" s="153" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E141" s="153" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F141" s="154" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G141" s="155" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H141" s="153" t="s">
         <v>13</v>
       </c>
       <c r="I141" s="153" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J141" s="153" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K141" s="153" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="L141" s="153" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M141" s="153" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="N141" s="153" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O141" s="149" t="s">
         <v>61</v>
       </c>
       <c r="P141" s="149" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -7109,7 +7106,7 @@
         <v>1</v>
       </c>
       <c r="I1" s="94" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J1" s="94" t="s">
         <v>14</v>
@@ -7118,19 +7115,19 @@
         <v>15</v>
       </c>
       <c r="L1" s="95" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="M1" s="95" t="s">
         <v>123</v>
       </c>
       <c r="N1" s="95" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="O1" s="95" t="s">
         <v>125</v>
       </c>
       <c r="P1" s="96" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q1" s="96" t="s">
         <v>103</v>
@@ -7165,10 +7162,10 @@
       </c>
       <c r="B2" s="100"/>
       <c r="C2" s="99" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2" s="99" t="s">
         <v>278</v>
-      </c>
-      <c r="D2" s="99" t="s">
-        <v>279</v>
       </c>
       <c r="E2" s="98" t="s">
         <v>10</v>
@@ -7186,13 +7183,13 @@
         <v>26</v>
       </c>
       <c r="J2" s="102" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K2" s="100" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L2" s="100" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M2" s="100" t="s">
         <v>33</v>
@@ -7201,10 +7198,10 @@
         <v>34</v>
       </c>
       <c r="O2" s="100" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P2" s="103" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Q2" s="100"/>
     </row>
@@ -7235,7 +7232,7 @@
         <v>13</v>
       </c>
       <c r="J3" s="102" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K3" s="102" t="s">
         <v>33</v>
@@ -7285,7 +7282,7 @@
         <v>13</v>
       </c>
       <c r="J4" s="102" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K4" s="102" t="s">
         <v>33</v>
@@ -7423,7 +7420,7 @@
         <v>58</v>
       </c>
       <c r="B7" s="113" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C7" s="114" t="s">
         <v>2</v>
@@ -7457,7 +7454,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="113" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C8" s="114" t="s">
         <v>2</v>
@@ -7557,7 +7554,7 @@
         <v>41</v>
       </c>
       <c r="B10" s="100" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C10" s="98" t="s">
         <v>42</v>
@@ -7584,7 +7581,7 @@
         <v>13</v>
       </c>
       <c r="K10" s="102" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L10" s="100" t="s">
         <v>33</v>
@@ -7631,7 +7628,7 @@
         <v>13</v>
       </c>
       <c r="L11" s="117" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M11" s="117" t="s">
         <v>33</v>
@@ -7702,7 +7699,7 @@
         <v>13</v>
       </c>
       <c r="K12" s="102" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L12" s="115"/>
       <c r="M12" s="91"/>
@@ -7746,7 +7743,7 @@
         <v>13</v>
       </c>
       <c r="K13" s="102" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L13" s="100" t="s">
         <v>33</v>
@@ -7813,7 +7810,7 @@
         <v>40</v>
       </c>
       <c r="B15" s="113" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C15" s="102" t="s">
         <v>2</v>
@@ -7839,7 +7836,7 @@
         <v>64</v>
       </c>
       <c r="B16" s="113" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C16" s="114" t="s">
         <v>2</v>
@@ -7923,7 +7920,7 @@
         <v>138</v>
       </c>
       <c r="B18" s="126" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C18" s="115" t="s">
         <v>66</v>
@@ -7985,7 +7982,7 @@
         <v>13</v>
       </c>
       <c r="J19" s="102" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K19" s="115" t="s">
         <v>33</v>
@@ -8265,7 +8262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -8293,10 +8290,10 @@
         <v>69</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>431</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>432</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>433</v>
       </c>
       <c r="D2" s="49"/>
     </row>
@@ -8305,10 +8302,10 @@
         <v>68</v>
       </c>
       <c r="B3" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>258</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>259</v>
       </c>
       <c r="D3" s="49"/>
     </row>
@@ -8320,19 +8317,19 @@
         <v>0</v>
       </c>
       <c r="C4" s="53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4" s="49"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>454</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>455</v>
       </c>
       <c r="D5" s="49"/>
     </row>
@@ -8341,82 +8338,82 @@
         <v>81</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>456</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>457</v>
       </c>
       <c r="D6" s="49"/>
     </row>
     <row r="7" spans="1:4" ht="15.6">
       <c r="A7" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B7" s="52" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D7" s="49"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="65" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B8" s="47" t="s">
+        <v>183</v>
+      </c>
+      <c r="C8" s="47" t="s">
         <v>184</v>
-      </c>
-      <c r="C8" s="47" t="s">
-        <v>185</v>
       </c>
       <c r="D8" s="49"/>
     </row>
     <row r="9" spans="1:4" ht="15.6">
       <c r="A9" s="64" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B9" s="52" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="65" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B10" s="84" t="s">
+        <v>448</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>449</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>450</v>
       </c>
       <c r="D10" s="49"/>
     </row>
     <row r="11" spans="1:4" ht="15.6">
       <c r="A11" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B11" s="54" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="62" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D11" s="49"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B12" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>258</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>259</v>
       </c>
       <c r="D12" s="49"/>
     </row>
@@ -8437,7 +8434,7 @@
         <v>30</v>
       </c>
       <c r="B14" s="68" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C14" s="48" t="s">
         <v>82</v>
@@ -8449,10 +8446,10 @@
         <v>31</v>
       </c>
       <c r="B15" s="68" t="s">
+        <v>181</v>
+      </c>
+      <c r="C15" s="48" t="s">
         <v>182</v>
-      </c>
-      <c r="C15" s="48" t="s">
-        <v>183</v>
       </c>
       <c r="D15" s="49"/>
     </row>
@@ -8492,8 +8489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -8504,7 +8501,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.6">
       <c r="A1" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>0</v>
@@ -8515,12 +8512,12 @@
         <v>131</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6">
       <c r="A3" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B3" s="52" t="s">
         <v>0</v>
@@ -8531,12 +8528,12 @@
         <v>132</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>145</v>
+        <v>431</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.6">
       <c r="A5" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" s="52" t="s">
         <v>0</v>
@@ -8544,7 +8541,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="66" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B6" s="47" t="s">
         <v>144</v>
@@ -8552,7 +8549,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.6">
       <c r="A7" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B7" s="52" t="s">
         <v>0</v>
@@ -8560,15 +8557,15 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="66" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B9" s="49">
         <v>30998801</v>
@@ -8642,10 +8639,10 @@
         <v>54</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="56"/>
@@ -8654,38 +8651,38 @@
     </row>
     <row r="3" spans="1:7" ht="15.6">
       <c r="A3" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>310</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>311</v>
       </c>
       <c r="F3" s="57"/>
       <c r="G3" s="57"/>
     </row>
     <row r="4" spans="1:7" ht="15.6">
       <c r="A4" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D4" s="87" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F4" s="57"/>
       <c r="G4" s="57"/>
@@ -8695,13 +8692,13 @@
         <v>133</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D5" s="87" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>55</v>
@@ -8711,13 +8708,13 @@
     </row>
     <row r="6" spans="1:7" ht="15.6">
       <c r="A6" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B6" s="52" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D6" s="54" t="s">
         <v>3</v>
@@ -8728,10 +8725,10 @@
     </row>
     <row r="7" spans="1:7" ht="17.399999999999999">
       <c r="A7" s="65" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C7" s="60"/>
       <c r="D7" s="49"/>
@@ -8741,16 +8738,16 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="65" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8" s="17" t="s">
+        <v>428</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>429</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="D8" s="50" t="s">
         <v>430</v>
-      </c>
-      <c r="D8" s="50" t="s">
-        <v>431</v>
       </c>
       <c r="E8" s="61"/>
       <c r="F8" s="49"/>
@@ -8758,7 +8755,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.6">
       <c r="A9" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B9" s="52" t="s">
         <v>0</v>
@@ -8767,7 +8764,7 @@
         <v>16</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E9" s="49"/>
       <c r="F9" s="49"/>
@@ -8775,16 +8772,16 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="66" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B10" s="17" t="s">
+        <v>436</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>452</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>437</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>453</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>438</v>
       </c>
       <c r="E10" s="49"/>
       <c r="F10" s="49"/>
@@ -8807,22 +8804,22 @@
     </row>
     <row r="12" spans="1:7" s="14" customFormat="1">
       <c r="A12" s="15" t="s">
+        <v>442</v>
+      </c>
+      <c r="B12" s="236" t="s">
         <v>443</v>
       </c>
-      <c r="B12" s="236" t="s">
+      <c r="C12" s="236" t="s">
         <v>444</v>
       </c>
-      <c r="C12" s="236" t="s">
-        <v>445</v>
-      </c>
       <c r="D12" s="47" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E12" s="47" t="s">
         <v>130</v>
       </c>
       <c r="F12" s="49" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G12" s="234"/>
     </row>
@@ -8831,10 +8828,10 @@
         <v>45</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="C13" s="48" t="s">
         <v>426</v>
-      </c>
-      <c r="C13" s="48" t="s">
-        <v>427</v>
       </c>
       <c r="D13" s="49"/>
       <c r="E13" s="49"/>
@@ -8843,34 +8840,34 @@
     </row>
     <row r="14" spans="1:7" s="21" customFormat="1" ht="15">
       <c r="A14" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="C14" s="48" t="s">
         <v>426</v>
       </c>
-      <c r="C14" s="48" t="s">
-        <v>427</v>
-      </c>
       <c r="D14" s="47" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E14" s="47" t="s">
         <v>130</v>
       </c>
       <c r="F14" s="49" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G14" s="49"/>
     </row>
     <row r="15" spans="1:7" ht="15.6">
       <c r="A15" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B15" s="52" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D15" s="54" t="s">
         <v>3</v>
@@ -8879,67 +8876,67 @@
         <v>4</v>
       </c>
       <c r="F15" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="G15" s="51" t="s">
         <v>168</v>
-      </c>
-      <c r="G15" s="51" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="66" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B16" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>437</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="D16" s="50" t="s">
         <v>438</v>
       </c>
-      <c r="D16" s="50" t="s">
+      <c r="E16" s="50" t="s">
         <v>439</v>
       </c>
-      <c r="E16" s="50" t="s">
+      <c r="F16" s="18" t="s">
         <v>440</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="G16" s="85" t="s">
         <v>441</v>
-      </c>
-      <c r="G16" s="85" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="B17" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="C17" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17" s="49" t="s">
         <v>171</v>
       </c>
-      <c r="C17" s="47" t="s">
-        <v>166</v>
-      </c>
-      <c r="D17" s="49" t="s">
+      <c r="E17" s="49" t="s">
+        <v>171</v>
+      </c>
+      <c r="F17" s="49" t="s">
+        <v>171</v>
+      </c>
+      <c r="G17" s="49" t="s">
         <v>172</v>
-      </c>
-      <c r="E17" s="49" t="s">
-        <v>172</v>
-      </c>
-      <c r="F17" s="49" t="s">
-        <v>172</v>
-      </c>
-      <c r="G17" s="49" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="21" customFormat="1" ht="15.6">
       <c r="A18" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B18" s="52" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D18" s="58"/>
       <c r="E18" s="237"/>
@@ -8948,13 +8945,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B19" s="236" t="s">
+        <v>443</v>
+      </c>
+      <c r="C19" s="236" t="s">
         <v>444</v>
-      </c>
-      <c r="C19" s="236" t="s">
-        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -9025,7 +9022,7 @@
         <v>93</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="14" customFormat="1" ht="16.8" thickBot="1">
@@ -9033,13 +9030,13 @@
         <v>32</v>
       </c>
       <c r="B2" s="232" t="s">
+        <v>433</v>
+      </c>
+      <c r="C2" s="68" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>434</v>
-      </c>
-      <c r="C2" s="68" t="s">
-        <v>267</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>435</v>
       </c>
       <c r="E2" s="56"/>
       <c r="F2" s="56"/>
@@ -9056,46 +9053,46 @@
         <v>80</v>
       </c>
       <c r="B3" s="232" t="s">
+        <v>433</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>266</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>434</v>
       </c>
-      <c r="C3" s="68" t="s">
-        <v>267</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>435</v>
-      </c>
       <c r="E3" s="192" t="s">
+        <v>213</v>
+      </c>
+      <c r="F3" s="81" t="s">
         <v>214</v>
       </c>
-      <c r="F3" s="81" t="s">
+      <c r="G3" s="192" t="s">
         <v>215</v>
-      </c>
-      <c r="G3" s="192" t="s">
-        <v>216</v>
       </c>
       <c r="H3" s="81" t="s">
         <v>39</v>
       </c>
       <c r="I3" s="206" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J3" s="233" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K3" s="233" t="s">
         <v>37</v>
       </c>
       <c r="L3" s="233" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M3" s="81" t="s">
         <v>20</v>
       </c>
       <c r="N3" s="233" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="O3" s="194" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="13.8" thickBot="1">
@@ -9103,28 +9100,28 @@
         <v>71</v>
       </c>
       <c r="B4" s="232" t="s">
+        <v>433</v>
+      </c>
+      <c r="C4" s="70" t="s">
+        <v>267</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>434</v>
-      </c>
-      <c r="C4" s="70" t="s">
-        <v>268</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>435</v>
       </c>
       <c r="E4" s="192" t="s">
         <v>101</v>
       </c>
       <c r="F4" s="81" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G4" s="208" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H4" s="208" t="s">
         <v>39</v>
       </c>
       <c r="I4" s="206" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J4" s="81">
         <v>6</v>
@@ -9142,7 +9139,7 @@
         <v>33332002</v>
       </c>
       <c r="O4" s="194" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -9238,7 +9235,7 @@
     </row>
     <row r="2" spans="1:15" s="196" customFormat="1" ht="16.2" thickBot="1">
       <c r="A2" s="202" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B2" s="203"/>
       <c r="C2" s="202"/>
@@ -9257,7 +9254,7 @@
     </row>
     <row r="3" spans="1:15" ht="13.8" thickBot="1">
       <c r="A3" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B3" s="191">
         <v>32001113</v>
@@ -9266,22 +9263,22 @@
         <v>2932598064</v>
       </c>
       <c r="D3" s="73" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E3" s="192" t="s">
+        <v>213</v>
+      </c>
+      <c r="F3" s="81" t="s">
         <v>214</v>
       </c>
-      <c r="F3" s="81" t="s">
+      <c r="G3" s="192" t="s">
         <v>215</v>
-      </c>
-      <c r="G3" s="192" t="s">
-        <v>216</v>
       </c>
       <c r="H3" s="81" t="s">
         <v>39</v>
       </c>
       <c r="I3" s="206" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J3" s="81">
         <v>6</v>
@@ -9299,12 +9296,12 @@
         <v>33332002</v>
       </c>
       <c r="O3" s="194" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="13.8" thickBot="1">
       <c r="A4" s="33" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B4" s="191">
         <v>32001113</v>
@@ -9313,7 +9310,7 @@
         <v>2932598064</v>
       </c>
       <c r="D4" s="73" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E4" s="192"/>
       <c r="F4" s="81"/>
@@ -9329,7 +9326,7 @@
     </row>
     <row r="5" spans="1:15" ht="13.8" thickBot="1">
       <c r="A5" s="33" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B5" s="191">
         <v>32001113</v>
@@ -9338,16 +9335,16 @@
         <v>2932598064</v>
       </c>
       <c r="D5" s="73" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E5" s="192" t="s">
+        <v>213</v>
+      </c>
+      <c r="F5" s="81" t="s">
         <v>214</v>
       </c>
-      <c r="F5" s="81" t="s">
+      <c r="G5" s="192" t="s">
         <v>215</v>
-      </c>
-      <c r="G5" s="192" t="s">
-        <v>216</v>
       </c>
       <c r="H5" s="81" t="s">
         <v>39</v>
@@ -9362,7 +9359,7 @@
     </row>
     <row r="6" spans="1:15" s="196" customFormat="1" ht="13.8" thickBot="1">
       <c r="A6" s="33" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B6" s="191">
         <v>32001113</v>
@@ -9371,7 +9368,7 @@
         <v>2932598064</v>
       </c>
       <c r="D6" s="81" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E6" s="192"/>
       <c r="F6" s="81"/>
@@ -9387,7 +9384,7 @@
     </row>
     <row r="7" spans="1:15" ht="13.8" thickBot="1">
       <c r="A7" s="33" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B7" s="191">
         <v>32001113</v>
@@ -9396,16 +9393,16 @@
         <v>2932598064</v>
       </c>
       <c r="D7" s="81" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E7" s="204" t="s">
         <v>101</v>
       </c>
       <c r="F7" s="204" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G7" s="204" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H7" s="81" t="s">
         <v>39</v>
@@ -9429,16 +9426,16 @@
         <v>2932598064</v>
       </c>
       <c r="D8" s="81" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E8" s="192" t="s">
+        <v>213</v>
+      </c>
+      <c r="F8" s="81" t="s">
         <v>214</v>
       </c>
-      <c r="F8" s="81" t="s">
+      <c r="G8" s="192" t="s">
         <v>215</v>
-      </c>
-      <c r="G8" s="192" t="s">
-        <v>216</v>
       </c>
       <c r="H8" s="81" t="s">
         <v>39</v>
@@ -9453,7 +9450,7 @@
     </row>
     <row r="9" spans="1:15" ht="16.2" thickBot="1">
       <c r="A9" s="202" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B9" s="203"/>
       <c r="C9" s="202"/>
@@ -9472,7 +9469,7 @@
     </row>
     <row r="10" spans="1:15" s="196" customFormat="1" ht="13.8" thickBot="1">
       <c r="A10" s="33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B10" s="191">
         <v>32001113</v>
@@ -9481,22 +9478,22 @@
         <v>2932598064</v>
       </c>
       <c r="D10" s="81" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E10" s="192" t="s">
+        <v>213</v>
+      </c>
+      <c r="F10" s="81" t="s">
         <v>214</v>
       </c>
-      <c r="F10" s="81" t="s">
+      <c r="G10" s="192" t="s">
         <v>215</v>
-      </c>
-      <c r="G10" s="192" t="s">
-        <v>216</v>
       </c>
       <c r="H10" s="81" t="s">
         <v>39</v>
       </c>
       <c r="I10" s="206" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J10" s="81">
         <v>6</v>
@@ -9514,12 +9511,12 @@
         <v>33332002</v>
       </c>
       <c r="O10" s="194" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="13.8" thickBot="1">
       <c r="A11" s="33" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B11" s="191">
         <v>32001113</v>
@@ -9528,7 +9525,7 @@
         <v>2932598064</v>
       </c>
       <c r="D11" s="81" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E11" s="192"/>
       <c r="F11" s="81"/>
@@ -9544,7 +9541,7 @@
     </row>
     <row r="12" spans="1:15" ht="13.8" thickBot="1">
       <c r="A12" s="33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B12" s="191">
         <v>32001113</v>
@@ -9553,7 +9550,7 @@
         <v>2932598064</v>
       </c>
       <c r="D12" s="81" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E12" s="192"/>
       <c r="F12" s="81"/>
@@ -9569,7 +9566,7 @@
     </row>
     <row r="13" spans="1:15" ht="13.8" thickBot="1">
       <c r="A13" s="33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B13" s="191">
         <v>32001113</v>
@@ -9578,22 +9575,22 @@
         <v>2932598064</v>
       </c>
       <c r="D13" s="81" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E13" s="192" t="s">
+        <v>213</v>
+      </c>
+      <c r="F13" s="81" t="s">
         <v>214</v>
       </c>
-      <c r="F13" s="81" t="s">
+      <c r="G13" s="192" t="s">
         <v>215</v>
-      </c>
-      <c r="G13" s="192" t="s">
-        <v>216</v>
       </c>
       <c r="H13" s="81" t="s">
         <v>39</v>
       </c>
       <c r="I13" s="206" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J13" s="81">
         <v>6</v>
@@ -9611,12 +9608,12 @@
         <v>33332002</v>
       </c>
       <c r="O13" s="194" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="16.2" thickBot="1">
       <c r="A14" s="202" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B14" s="203"/>
       <c r="C14" s="202"/>
@@ -9644,7 +9641,7 @@
         <v>2932598064</v>
       </c>
       <c r="D15" s="81" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E15" s="192"/>
       <c r="F15" s="81"/>
@@ -9660,7 +9657,7 @@
     </row>
     <row r="16" spans="1:15" ht="13.8" thickBot="1">
       <c r="A16" s="33" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B16" s="191">
         <v>32001113</v>
@@ -9669,7 +9666,7 @@
         <v>2932598064</v>
       </c>
       <c r="D16" s="81" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E16" s="81"/>
       <c r="F16" s="81"/>
@@ -9685,7 +9682,7 @@
     </row>
     <row r="17" spans="1:15" ht="13.8" thickBot="1">
       <c r="A17" s="33" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B17" s="191">
         <v>32001113</v>
@@ -9694,16 +9691,16 @@
         <v>2932598064</v>
       </c>
       <c r="D17" s="81" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E17" s="192" t="s">
+        <v>213</v>
+      </c>
+      <c r="F17" s="81" t="s">
         <v>214</v>
       </c>
-      <c r="F17" s="81" t="s">
+      <c r="G17" s="192" t="s">
         <v>215</v>
-      </c>
-      <c r="G17" s="192" t="s">
-        <v>216</v>
       </c>
       <c r="H17" s="81" t="s">
         <v>39</v>
@@ -9718,7 +9715,7 @@
     </row>
     <row r="18" spans="1:15" ht="13.8" thickBot="1">
       <c r="A18" s="33" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B18" s="191">
         <v>32001113</v>
@@ -9727,7 +9724,7 @@
         <v>2932598064</v>
       </c>
       <c r="D18" s="81" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E18" s="33"/>
       <c r="F18" s="33"/>
@@ -9737,7 +9734,7 @@
     </row>
     <row r="19" spans="1:15" ht="13.8" thickBot="1">
       <c r="A19" s="33" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B19" s="191">
         <v>32001113</v>
@@ -9746,16 +9743,16 @@
         <v>2932598064</v>
       </c>
       <c r="D19" s="81" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E19" s="204" t="s">
         <v>101</v>
       </c>
       <c r="F19" s="204" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G19" s="204" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H19" s="81" t="s">
         <v>39</v>
@@ -9810,49 +9807,49 @@
     </row>
     <row r="21" spans="1:15" ht="13.8" thickBot="1">
       <c r="A21" s="238" t="s">
+        <v>447</v>
+      </c>
+      <c r="B21" s="239" t="s">
         <v>448</v>
       </c>
-      <c r="B21" s="239" t="s">
+      <c r="C21" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>451</v>
-      </c>
       <c r="E21" s="240" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F21" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="G21" s="241" t="s">
         <v>215</v>
-      </c>
-      <c r="G21" s="241" t="s">
-        <v>216</v>
       </c>
       <c r="H21" s="206" t="s">
         <v>39</v>
       </c>
       <c r="I21" s="233" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J21" s="233" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K21" s="233" t="s">
         <v>62</v>
       </c>
       <c r="L21" s="233" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M21" s="242" t="s">
         <v>20</v>
       </c>
       <c r="N21" s="243" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -9893,7 +9890,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>87</v>
@@ -9934,13 +9931,13 @@
         <v>23</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>406</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>407</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="86" t="s">
         <v>408</v>
-      </c>
-      <c r="D2" s="86" t="s">
-        <v>409</v>
       </c>
       <c r="E2" s="19"/>
       <c r="F2" s="14"/>
@@ -9959,13 +9956,13 @@
         <v>24</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="D3" s="86" t="s">
         <v>305</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>307</v>
-      </c>
-      <c r="D3" s="86" t="s">
-        <v>306</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="14"/>
@@ -9984,22 +9981,22 @@
         <v>105</v>
       </c>
       <c r="B4" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="D4" s="86" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>307</v>
-      </c>
-      <c r="D4" s="86" t="s">
-        <v>306</v>
-      </c>
       <c r="E4" s="72" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>59</v>
       </c>
       <c r="G4" s="72" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>39</v>
@@ -10020,7 +10017,7 @@
         <v>20</v>
       </c>
       <c r="N4" s="16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="O4" s="13" t="s">
         <v>73</v>
@@ -10028,25 +10025,25 @@
     </row>
     <row r="5" spans="1:15" ht="15">
       <c r="A5" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B5" s="16" t="s">
+        <v>406</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>407</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="D5" s="86" t="s">
         <v>408</v>
       </c>
-      <c r="D5" s="86" t="s">
-        <v>409</v>
-      </c>
       <c r="E5" s="72" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="72" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>39</v>
@@ -10067,7 +10064,7 @@
         <v>20</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="O5" s="13" t="s">
         <v>73</v>

</xml_diff>